<commit_message>
file handling and maps
</commit_message>
<xml_diff>
--- a/src/com/syntax/utils/Test.xlsx
+++ b/src/com/syntax/utils/Test.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/puskaruprety/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/puskaruprety/eclipse_workplace/JavaBasics/src/com/syntax/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5129A15B-E131-2242-9AB1-27F489D2462E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266BA57A-58F3-964F-B541-AB0BCD66226E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{6BB5A7B2-8CD6-2F47-8562-FE96C9736A4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>First Name</t>
   </si>
@@ -44,16 +45,73 @@
     <t>Last Name</t>
   </si>
   <si>
-    <t>Hobby</t>
-  </si>
-  <si>
     <t>Oscar</t>
   </si>
   <si>
     <t>Patel</t>
   </si>
   <si>
-    <t>Gamming</t>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Teskyer</t>
+  </si>
+  <si>
+    <t>sharma</t>
+  </si>
+  <si>
+    <t>johnson</t>
+  </si>
+  <si>
+    <t>johnso</t>
+  </si>
+  <si>
+    <t>Janel</t>
+  </si>
+  <si>
+    <t>Tokeyo</t>
+  </si>
+  <si>
+    <t>Cool</t>
+  </si>
+  <si>
+    <t>Boy</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Thakkar</t>
+  </si>
+  <si>
+    <t>Prashuv</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Aaditya</t>
+  </si>
+  <si>
+    <t>Dhakal</t>
+  </si>
+  <si>
+    <t>Rabi</t>
+  </si>
+  <si>
+    <t>Lamichhane</t>
   </si>
 </sst>
 </file>
@@ -89,8 +147,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,15 +464,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CFB33D-CB0B-754E-BBCD-20D86A8BCAD1}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,18 +480,168 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>32</v>
+      </c>
+      <c r="D3">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>87000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>85000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>48</v>
+      </c>
+      <c r="D6">
+        <v>100000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D22A676-9D40-C04D-85B0-149D6F461C9D}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>657584848</v>
+      </c>
+      <c r="D2" s="1">
+        <v>36142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>4343434434</v>
+      </c>
+      <c r="D3" s="1">
+        <v>29283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>3232323234</v>
+      </c>
+      <c r="D4" s="1">
+        <v>33948</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>3232434545</v>
+      </c>
+      <c r="D5" s="1">
+        <v>34369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>